<commit_message>
0522 modifiy query and  save excel value to db
</commit_message>
<xml_diff>
--- a/backend/private/db/analysis/이미지_속성_최종.xlsx
+++ b/backend/private/db/analysis/이미지_속성_최종.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\study\Subject\Software Capstone\Project\문서\이미지 속성\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53ED77DE-87E9-42ED-BAD4-1BD86C1E778B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA72335-07F5-4BFE-92AE-A6620CB4AB0F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{0D4B19A7-728F-4523-98BD-6CF286C421CB}"/>
+    <workbookView xWindow="4764" yWindow="2412" windowWidth="17280" windowHeight="8964" xr2:uid="{0D4B19A7-728F-4523-98BD-6CF286C421CB}"/>
   </bookViews>
   <sheets>
-    <sheet name="남자" sheetId="1" r:id="rId1"/>
-    <sheet name="여자" sheetId="2" r:id="rId2"/>
+    <sheet name="setting" sheetId="3" r:id="rId1"/>
+    <sheet name="1" sheetId="1" r:id="rId2"/>
+    <sheet name="2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1421" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1425" uniqueCount="292">
   <si>
     <t>머리길이</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -742,10 +743,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>김소현</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>장발</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -762,54 +759,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>김유정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>예리</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>쯔위</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>엠버허드</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>섹시</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>니콜키드먼</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>단발</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>드류베이모어</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>스칼렛요한슨</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>아만다사이프리드</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>엠마왓슨</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>미란다커</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">장발 </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -826,363 +783,423 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>바바라팔빈</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>제시카스탐</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>헤더막스</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>김태희</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>문채원</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>미나</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>단아</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>박신혜</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>서은수</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>서현진</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>설현</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>손나은</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>솔라</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>신세경</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>오하영</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>윤아</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>이연희</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>이영애</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>장원영</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>전지현</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>정은지</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>한지민</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>한효주</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>화사</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>나탈리도메르</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>레베카퍼거슨</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>메간폭스</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>밀라요보비치</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>샤를리즈테론</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>안젤리나졸리</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>안렉산드라다드다리오</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>앤해서웨이</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>에바그린</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>엘리자베스올슨</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>제니퍼로렌스</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>제시카알바</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>케이트윈슬렛</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>크리스틴스튜어트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>클로이모레츠</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>키이라나이틀리</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>테레사팔머</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>경리</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>구혜선</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>나나</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>나연</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>낸시</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>박하선</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>사나</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>설리</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>소진</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>손예진</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>아이유</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>연우</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>이민정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>전소민</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>전효성</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>정연</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>제니</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>조이</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>주결경</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>지효</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>채영</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>초이</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>크리스탈</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>하니</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>한가인</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>혜리</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>나탈리포트만</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>레이첼맥아담스</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>릴리콜린스</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>밀라쿠니스</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>바네사허진스</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>시얼샤로넌</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>안나켄드릭</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>엘르패닝</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>올리비아와일드</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>헤일리스타인펠드</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>갤가돗</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>다코타존슨</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>데이지리들리</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>드류베리모어</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>디피카파두콘</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>마고로비</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>모레나바카린</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>블레이크라이블리</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>애밀리블런트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>조이살다나</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>줄리아로버츠</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>캐서린헤이글</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>엠마스톤</t>
+    <t>김소현.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>김유정.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>예리.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>엠마스톤.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>캐서린헤이글.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>줄리아로버츠.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>조이살다나.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>애밀리블런트.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>블레이크라이블리.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모레나바카린.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마고로비.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>디피카파두콘.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>드류베리모어.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>데이지리들리.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>다코타존슨.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>갤가돗.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>헤일리스타인펠드.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>올리비아와일드.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>엘르패닝.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>안나켄드릭.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시얼샤로넌.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>바네사허진스.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>밀라쿠니스.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>릴리콜린스.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>레이첼맥아담스.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>나탈리포트만.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>혜리.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>한가인.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>하니.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>크리스탈.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>초이.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>채영.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지효.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주결경.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>조이.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>제니.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>정연.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전효성.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전소민.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이민정.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>연우.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이유.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>손예진.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>소진.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>설리.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사나.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>박하선.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>낸시.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>나연.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>나나.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>구혜선.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>경리.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>테레사팔머.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>키이라나이틀리.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>클로이모레츠.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>크리스틴스튜어트.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>케이트윈슬렛.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>제시카알바.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>제니퍼로렌스.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>엘리자베스올슨.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>에바그린.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>쯔위.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>엠버허드.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>니콜키드먼.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>드류베이모어.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스칼렛요한슨.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>앤해서웨이.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>안렉산드라다드다리오.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>안젤리나졸리.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>샤를리즈테론.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>밀라요보비치.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>메간폭스.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>레베카퍼거슨.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>나탈리도메르.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>화사.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>한효주.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>한지민.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>정은지.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전지현.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>장원영.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이영애.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이연희.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>윤아.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오하영.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>신세경.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>솔라.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>손나은.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>설현.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서현진.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서은수.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>박신혜.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>미나.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>문채원.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>김태희.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>헤더막스.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>제시카스탐.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>바바라팔빈.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>미란다커.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>엠마왓슨.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아만다사이프리드.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>folder name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sheet name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>analysis_man</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>analysis_woman</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1546,11 +1563,55 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBCEA11C-9251-44E7-AA41-F0DC5DACB4A0}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="2" max="2" width="12.3984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>291</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7DEA72E-EEE8-405E-88CB-70883EC1F59F}">
   <dimension ref="B1:H102"/>
   <sheetViews>
-    <sheetView topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="B103" sqref="B103"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -3917,17 +3978,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F3E1D40-E48E-44C9-9049-1BB7413AF33F}">
   <dimension ref="B2:H102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="D108" sqref="D108"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="11.09765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.09765625" customWidth="1"/>
     <col min="3" max="3" width="12.59765625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.5" bestFit="1" customWidth="1"/>
@@ -3961,10 +4022,10 @@
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B3" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="C3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D3" t="s">
         <v>21</v>
@@ -3973,21 +4034,21 @@
         <v>31</v>
       </c>
       <c r="F3" t="s">
+        <v>178</v>
+      </c>
+      <c r="G3" t="s">
         <v>179</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>180</v>
-      </c>
-      <c r="H3" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="C4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D4" t="s">
         <v>14</v>
@@ -4002,15 +4063,15 @@
         <v>16</v>
       </c>
       <c r="H4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="C5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D5" t="s">
         <v>14</v>
@@ -4025,15 +4086,15 @@
         <v>16</v>
       </c>
       <c r="H5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
-        <v>184</v>
+        <v>249</v>
       </c>
       <c r="C6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D6" t="s">
         <v>14</v>
@@ -4048,15 +4109,15 @@
         <v>16</v>
       </c>
       <c r="H6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B7" t="s">
-        <v>185</v>
+        <v>250</v>
       </c>
       <c r="C7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D7" t="s">
         <v>14</v>
@@ -4065,21 +4126,21 @@
         <v>27</v>
       </c>
       <c r="F7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G7" t="s">
         <v>24</v>
       </c>
       <c r="H7" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B8" t="s">
-        <v>187</v>
+        <v>251</v>
       </c>
       <c r="C8" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="D8" t="s">
         <v>23</v>
@@ -4099,10 +4160,10 @@
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B9" t="s">
-        <v>189</v>
+        <v>252</v>
       </c>
       <c r="C9" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="D9" t="s">
         <v>14</v>
@@ -4117,15 +4178,15 @@
         <v>24</v>
       </c>
       <c r="H9" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B10" t="s">
-        <v>190</v>
+        <v>253</v>
       </c>
       <c r="C10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D10" t="s">
         <v>14</v>
@@ -4140,15 +4201,15 @@
         <v>24</v>
       </c>
       <c r="H10" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B11" t="s">
-        <v>191</v>
+        <v>287</v>
       </c>
       <c r="C11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D11" t="s">
         <v>23</v>
@@ -4163,15 +4224,15 @@
         <v>24</v>
       </c>
       <c r="H11" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B12" t="s">
-        <v>192</v>
+        <v>286</v>
       </c>
       <c r="C12" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="D12" t="s">
         <v>23</v>
@@ -4186,21 +4247,21 @@
         <v>24</v>
       </c>
       <c r="H12" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B13" t="s">
-        <v>193</v>
+        <v>285</v>
       </c>
       <c r="C13" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="D13" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="E13" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="F13" t="s">
         <v>28</v>
@@ -4209,15 +4270,15 @@
         <v>24</v>
       </c>
       <c r="H13" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B14" t="s">
-        <v>198</v>
+        <v>284</v>
       </c>
       <c r="C14" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D14" t="s">
         <v>14</v>
@@ -4232,15 +4293,15 @@
         <v>24</v>
       </c>
       <c r="H14" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B15" t="s">
-        <v>199</v>
+        <v>283</v>
       </c>
       <c r="C15" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D15" t="s">
         <v>23</v>
@@ -4260,10 +4321,10 @@
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B16" t="s">
-        <v>200</v>
+        <v>282</v>
       </c>
       <c r="C16" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D16" t="s">
         <v>14</v>
@@ -4278,15 +4339,15 @@
         <v>24</v>
       </c>
       <c r="H16" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B17" t="s">
-        <v>201</v>
+        <v>281</v>
       </c>
       <c r="C17" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D17" t="s">
         <v>14</v>
@@ -4301,15 +4362,15 @@
         <v>16</v>
       </c>
       <c r="H17" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B18" t="s">
-        <v>202</v>
+        <v>280</v>
       </c>
       <c r="C18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D18" t="s">
         <v>14</v>
@@ -4324,15 +4385,15 @@
         <v>16</v>
       </c>
       <c r="H18" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B19" t="s">
-        <v>203</v>
+        <v>279</v>
       </c>
       <c r="C19" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D19" t="s">
         <v>14</v>
@@ -4347,15 +4408,15 @@
         <v>16</v>
       </c>
       <c r="H19" t="s">
-        <v>204</v>
+        <v>187</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B20" t="s">
-        <v>205</v>
+        <v>278</v>
       </c>
       <c r="C20" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D20" t="s">
         <v>14</v>
@@ -4370,15 +4431,15 @@
         <v>16</v>
       </c>
       <c r="H20" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B21" t="s">
-        <v>206</v>
+        <v>277</v>
       </c>
       <c r="C21" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D21" t="s">
         <v>21</v>
@@ -4393,15 +4454,15 @@
         <v>16</v>
       </c>
       <c r="H21" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B22" t="s">
-        <v>207</v>
+        <v>276</v>
       </c>
       <c r="C22" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D22" t="s">
         <v>14</v>
@@ -4416,15 +4477,15 @@
         <v>16</v>
       </c>
       <c r="H22" t="s">
-        <v>204</v>
+        <v>187</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B23" t="s">
-        <v>208</v>
+        <v>275</v>
       </c>
       <c r="C23" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D23" t="s">
         <v>14</v>
@@ -4439,15 +4500,15 @@
         <v>16</v>
       </c>
       <c r="H23" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B24" t="s">
-        <v>209</v>
+        <v>274</v>
       </c>
       <c r="C24" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D24" t="s">
         <v>14</v>
@@ -4462,15 +4523,15 @@
         <v>16</v>
       </c>
       <c r="H24" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B25" t="s">
-        <v>210</v>
+        <v>273</v>
       </c>
       <c r="C25" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D25" t="s">
         <v>14</v>
@@ -4485,15 +4546,15 @@
         <v>16</v>
       </c>
       <c r="H25" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B26" t="s">
-        <v>211</v>
+        <v>272</v>
       </c>
       <c r="C26" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D26" t="s">
         <v>14</v>
@@ -4508,15 +4569,15 @@
         <v>16</v>
       </c>
       <c r="H26" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B27" t="s">
-        <v>212</v>
+        <v>271</v>
       </c>
       <c r="C27" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D27" t="s">
         <v>21</v>
@@ -4531,15 +4592,15 @@
         <v>16</v>
       </c>
       <c r="H27" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B28" t="s">
-        <v>213</v>
+        <v>270</v>
       </c>
       <c r="C28" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D28" t="s">
         <v>14</v>
@@ -4554,15 +4615,15 @@
         <v>16</v>
       </c>
       <c r="H28" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B29" t="s">
-        <v>214</v>
+        <v>269</v>
       </c>
       <c r="C29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D29" t="s">
         <v>14</v>
@@ -4577,15 +4638,15 @@
         <v>16</v>
       </c>
       <c r="H29" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B30" t="s">
-        <v>215</v>
+        <v>268</v>
       </c>
       <c r="C30" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D30" t="s">
         <v>14</v>
@@ -4600,15 +4661,15 @@
         <v>16</v>
       </c>
       <c r="H30" t="s">
-        <v>204</v>
+        <v>187</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B31" t="s">
-        <v>216</v>
+        <v>267</v>
       </c>
       <c r="C31" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D31" t="s">
         <v>14</v>
@@ -4623,15 +4684,15 @@
         <v>16</v>
       </c>
       <c r="H31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B32" t="s">
-        <v>217</v>
+        <v>266</v>
       </c>
       <c r="C32" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D32" t="s">
         <v>14</v>
@@ -4646,15 +4707,15 @@
         <v>16</v>
       </c>
       <c r="H32" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B33" t="s">
-        <v>218</v>
+        <v>265</v>
       </c>
       <c r="C33" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D33" t="s">
         <v>21</v>
@@ -4669,12 +4730,12 @@
         <v>16</v>
       </c>
       <c r="H33" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B34" t="s">
-        <v>219</v>
+        <v>264</v>
       </c>
       <c r="C34" t="s">
         <v>15</v>
@@ -4692,15 +4753,15 @@
         <v>16</v>
       </c>
       <c r="H34" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B35" t="s">
-        <v>220</v>
+        <v>263</v>
       </c>
       <c r="C35" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D35" t="s">
         <v>14</v>
@@ -4715,15 +4776,15 @@
         <v>16</v>
       </c>
       <c r="H35" t="s">
-        <v>204</v>
+        <v>187</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B36" t="s">
-        <v>221</v>
+        <v>262</v>
       </c>
       <c r="C36" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D36" t="s">
         <v>14</v>
@@ -4743,10 +4804,10 @@
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B37" t="s">
-        <v>222</v>
+        <v>261</v>
       </c>
       <c r="C37" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="D37" t="s">
         <v>23</v>
@@ -4761,15 +4822,15 @@
         <v>24</v>
       </c>
       <c r="H37" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B38" t="s">
-        <v>223</v>
+        <v>260</v>
       </c>
       <c r="C38" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="D38" t="s">
         <v>23</v>
@@ -4784,15 +4845,15 @@
         <v>24</v>
       </c>
       <c r="H38" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B39" t="s">
-        <v>224</v>
+        <v>259</v>
       </c>
       <c r="C39" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D39" t="s">
         <v>23</v>
@@ -4807,15 +4868,15 @@
         <v>24</v>
       </c>
       <c r="H39" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B40" t="s">
-        <v>225</v>
+        <v>258</v>
       </c>
       <c r="C40" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="D40" t="s">
         <v>21</v>
@@ -4835,10 +4896,10 @@
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B41" t="s">
-        <v>226</v>
+        <v>257</v>
       </c>
       <c r="C41" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D41" t="s">
         <v>23</v>
@@ -4853,15 +4914,15 @@
         <v>24</v>
       </c>
       <c r="H41" t="s">
-        <v>204</v>
+        <v>187</v>
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B42" t="s">
-        <v>227</v>
+        <v>256</v>
       </c>
       <c r="C42" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D42" t="s">
         <v>14</v>
@@ -4881,10 +4942,10 @@
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B43" t="s">
-        <v>228</v>
+        <v>255</v>
       </c>
       <c r="C43" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D43" t="s">
         <v>14</v>
@@ -4899,15 +4960,15 @@
         <v>24</v>
       </c>
       <c r="H43" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B44" t="s">
-        <v>229</v>
+        <v>254</v>
       </c>
       <c r="C44" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D44" t="s">
         <v>14</v>
@@ -4922,15 +4983,15 @@
         <v>24</v>
       </c>
       <c r="H44" t="s">
-        <v>204</v>
+        <v>187</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B45" t="s">
-        <v>230</v>
+        <v>248</v>
       </c>
       <c r="C45" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="D45" t="s">
         <v>23</v>
@@ -4945,15 +5006,15 @@
         <v>24</v>
       </c>
       <c r="H45" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B46" t="s">
-        <v>231</v>
+        <v>247</v>
       </c>
       <c r="C46" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D46" t="s">
         <v>14</v>
@@ -4968,15 +5029,15 @@
         <v>24</v>
       </c>
       <c r="H46" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B47" t="s">
-        <v>232</v>
+        <v>246</v>
       </c>
       <c r="C47" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="D47" t="s">
         <v>14</v>
@@ -4991,15 +5052,15 @@
         <v>24</v>
       </c>
       <c r="H47" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B48" t="s">
-        <v>233</v>
+        <v>245</v>
       </c>
       <c r="C48" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="D48" t="s">
         <v>21</v>
@@ -5014,15 +5075,15 @@
         <v>24</v>
       </c>
       <c r="H48" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B49" t="s">
-        <v>234</v>
+        <v>244</v>
       </c>
       <c r="C49" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="D49" t="s">
         <v>23</v>
@@ -5037,15 +5098,15 @@
         <v>24</v>
       </c>
       <c r="H49" t="s">
-        <v>204</v>
+        <v>187</v>
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B50" t="s">
-        <v>235</v>
+        <v>243</v>
       </c>
       <c r="C50" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D50" t="s">
         <v>14</v>
@@ -5060,15 +5121,15 @@
         <v>24</v>
       </c>
       <c r="H50" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B51" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="C51" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D51" t="s">
         <v>14</v>
@@ -5083,15 +5144,15 @@
         <v>24</v>
       </c>
       <c r="H51" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B52" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="C52" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D52" t="s">
         <v>21</v>
@@ -5106,15 +5167,15 @@
         <v>24</v>
       </c>
       <c r="H52" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B53" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="C53" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D53" t="s">
         <v>14</v>
@@ -5129,7 +5190,7 @@
         <v>24</v>
       </c>
       <c r="H53" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.4">
@@ -5137,7 +5198,7 @@
         <v>239</v>
       </c>
       <c r="C54" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D54" t="s">
         <v>14</v>
@@ -5152,15 +5213,15 @@
         <v>16</v>
       </c>
       <c r="H54" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B55" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C55" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D55" t="s">
         <v>21</v>
@@ -5175,15 +5236,15 @@
         <v>16</v>
       </c>
       <c r="H55" t="s">
-        <v>204</v>
+        <v>187</v>
       </c>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B56" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="C56" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D56" t="s">
         <v>14</v>
@@ -5198,15 +5259,15 @@
         <v>16</v>
       </c>
       <c r="H56" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="57" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B57" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="C57" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D57" t="s">
         <v>21</v>
@@ -5221,15 +5282,15 @@
         <v>16</v>
       </c>
       <c r="H57" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B58" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="C58" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D58" t="s">
         <v>14</v>
@@ -5244,15 +5305,15 @@
         <v>16</v>
       </c>
       <c r="H58" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B59" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="C59" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D59" t="s">
         <v>21</v>
@@ -5267,15 +5328,15 @@
         <v>16</v>
       </c>
       <c r="H59" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B60" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
       <c r="C60" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D60" t="s">
         <v>23</v>
@@ -5290,15 +5351,15 @@
         <v>16</v>
       </c>
       <c r="H60" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B61" t="s">
-        <v>246</v>
+        <v>232</v>
       </c>
       <c r="C61" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="D61" t="s">
         <v>14</v>
@@ -5313,15 +5374,15 @@
         <v>16</v>
       </c>
       <c r="H61" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B62" t="s">
-        <v>247</v>
+        <v>231</v>
       </c>
       <c r="C62" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D62" t="s">
         <v>14</v>
@@ -5336,15 +5397,15 @@
         <v>16</v>
       </c>
       <c r="H62" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B63" t="s">
-        <v>248</v>
+        <v>230</v>
       </c>
       <c r="C63" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="D63" t="s">
         <v>14</v>
@@ -5359,15 +5420,15 @@
         <v>16</v>
       </c>
       <c r="H63" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="64" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B64" t="s">
-        <v>249</v>
+        <v>229</v>
       </c>
       <c r="C64" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D64" t="s">
         <v>14</v>
@@ -5382,15 +5443,15 @@
         <v>16</v>
       </c>
       <c r="H64" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="65" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B65" t="s">
-        <v>250</v>
+        <v>228</v>
       </c>
       <c r="C65" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D65" t="s">
         <v>14</v>
@@ -5405,15 +5466,15 @@
         <v>16</v>
       </c>
       <c r="H65" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="66" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B66" t="s">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="C66" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D66" t="s">
         <v>14</v>
@@ -5428,15 +5489,15 @@
         <v>16</v>
       </c>
       <c r="H66" t="s">
-        <v>204</v>
+        <v>187</v>
       </c>
     </row>
     <row r="67" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B67" t="s">
-        <v>252</v>
+        <v>226</v>
       </c>
       <c r="C67" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="D67" t="s">
         <v>14</v>
@@ -5451,15 +5512,15 @@
         <v>16</v>
       </c>
       <c r="H67" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="68" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B68" t="s">
-        <v>253</v>
+        <v>225</v>
       </c>
       <c r="C68" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D68" t="s">
         <v>21</v>
@@ -5474,15 +5535,15 @@
         <v>16</v>
       </c>
       <c r="H68" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="69" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B69" t="s">
-        <v>254</v>
+        <v>224</v>
       </c>
       <c r="C69" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="D69" t="s">
         <v>21</v>
@@ -5497,15 +5558,15 @@
         <v>16</v>
       </c>
       <c r="H69" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="70" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B70" t="s">
-        <v>255</v>
+        <v>223</v>
       </c>
       <c r="C70" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D70" t="s">
         <v>14</v>
@@ -5520,15 +5581,15 @@
         <v>16</v>
       </c>
       <c r="H70" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="71" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B71" t="s">
-        <v>256</v>
+        <v>222</v>
       </c>
       <c r="C71" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D71" t="s">
         <v>14</v>
@@ -5543,15 +5604,15 @@
         <v>16</v>
       </c>
       <c r="H71" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="72" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B72" t="s">
-        <v>257</v>
+        <v>221</v>
       </c>
       <c r="C72" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D72" t="s">
         <v>14</v>
@@ -5566,15 +5627,15 @@
         <v>16</v>
       </c>
       <c r="H72" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="73" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B73" t="s">
-        <v>258</v>
+        <v>220</v>
       </c>
       <c r="C73" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D73" t="s">
         <v>21</v>
@@ -5589,15 +5650,15 @@
         <v>16</v>
       </c>
       <c r="H73" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="74" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B74" t="s">
-        <v>259</v>
+        <v>219</v>
       </c>
       <c r="C74" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D74" t="s">
         <v>14</v>
@@ -5612,15 +5673,15 @@
         <v>16</v>
       </c>
       <c r="H74" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="75" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B75" t="s">
-        <v>260</v>
+        <v>218</v>
       </c>
       <c r="C75" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="D75" t="s">
         <v>14</v>
@@ -5635,15 +5696,15 @@
         <v>16</v>
       </c>
       <c r="H75" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="76" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B76" t="s">
-        <v>261</v>
+        <v>217</v>
       </c>
       <c r="C76" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D76" t="s">
         <v>14</v>
@@ -5658,15 +5719,15 @@
         <v>16</v>
       </c>
       <c r="H76" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="77" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B77" t="s">
-        <v>262</v>
+        <v>216</v>
       </c>
       <c r="C77" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D77" t="s">
         <v>21</v>
@@ -5681,15 +5742,15 @@
         <v>16</v>
       </c>
       <c r="H77" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="78" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B78" t="s">
-        <v>263</v>
+        <v>215</v>
       </c>
       <c r="C78" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D78" t="s">
         <v>14</v>
@@ -5704,15 +5765,15 @@
         <v>16</v>
       </c>
       <c r="H78" t="s">
-        <v>204</v>
+        <v>187</v>
       </c>
     </row>
     <row r="79" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B79" t="s">
-        <v>264</v>
+        <v>214</v>
       </c>
       <c r="C79" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D79" t="s">
         <v>14</v>
@@ -5727,15 +5788,15 @@
         <v>16</v>
       </c>
       <c r="H79" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="80" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B80" t="s">
-        <v>265</v>
+        <v>213</v>
       </c>
       <c r="C80" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D80" t="s">
         <v>14</v>
@@ -5750,15 +5811,15 @@
         <v>24</v>
       </c>
       <c r="H80" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="81" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B81" t="s">
-        <v>266</v>
+        <v>212</v>
       </c>
       <c r="C81" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D81" t="s">
         <v>14</v>
@@ -5773,15 +5834,15 @@
         <v>24</v>
       </c>
       <c r="H81" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="82" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B82" t="s">
-        <v>267</v>
+        <v>211</v>
       </c>
       <c r="C82" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D82" t="s">
         <v>14</v>
@@ -5796,15 +5857,15 @@
         <v>24</v>
       </c>
       <c r="H82" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="83" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B83" t="s">
-        <v>268</v>
+        <v>210</v>
       </c>
       <c r="C83" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D83" t="s">
         <v>14</v>
@@ -5819,15 +5880,15 @@
         <v>24</v>
       </c>
       <c r="H83" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="84" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B84" t="s">
-        <v>269</v>
+        <v>209</v>
       </c>
       <c r="C84" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D84" t="s">
         <v>14</v>
@@ -5842,15 +5903,15 @@
         <v>24</v>
       </c>
       <c r="H84" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="85" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B85" t="s">
-        <v>270</v>
+        <v>208</v>
       </c>
       <c r="C85" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="D85" t="s">
         <v>14</v>
@@ -5865,15 +5926,15 @@
         <v>24</v>
       </c>
       <c r="H85" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="86" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B86" t="s">
-        <v>271</v>
+        <v>207</v>
       </c>
       <c r="C86" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D86" t="s">
         <v>14</v>
@@ -5888,15 +5949,15 @@
         <v>24</v>
       </c>
       <c r="H86" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="87" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B87" t="s">
-        <v>272</v>
+        <v>206</v>
       </c>
       <c r="C87" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D87" t="s">
         <v>14</v>
@@ -5911,15 +5972,15 @@
         <v>24</v>
       </c>
       <c r="H87" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="88" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B88" t="s">
-        <v>273</v>
+        <v>205</v>
       </c>
       <c r="C88" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D88" t="s">
         <v>23</v>
@@ -5934,15 +5995,15 @@
         <v>24</v>
       </c>
       <c r="H88" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="89" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B89" t="s">
-        <v>274</v>
+        <v>204</v>
       </c>
       <c r="C89" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D89" t="s">
         <v>14</v>
@@ -5957,15 +6018,15 @@
         <v>24</v>
       </c>
       <c r="H89" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="90" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B90" t="s">
-        <v>275</v>
+        <v>203</v>
       </c>
       <c r="C90" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D90" t="s">
         <v>14</v>
@@ -5980,15 +6041,15 @@
         <v>24</v>
       </c>
       <c r="H90" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="91" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B91" t="s">
-        <v>276</v>
+        <v>202</v>
       </c>
       <c r="C91" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D91" t="s">
         <v>21</v>
@@ -6003,15 +6064,15 @@
         <v>24</v>
       </c>
       <c r="H91" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="92" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B92" t="s">
-        <v>277</v>
+        <v>201</v>
       </c>
       <c r="C92" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D92" t="s">
         <v>14</v>
@@ -6026,15 +6087,15 @@
         <v>24</v>
       </c>
       <c r="H92" t="s">
-        <v>204</v>
+        <v>187</v>
       </c>
     </row>
     <row r="93" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B93" t="s">
-        <v>278</v>
+        <v>200</v>
       </c>
       <c r="C93" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D93" t="s">
         <v>23</v>
@@ -6049,15 +6110,15 @@
         <v>24</v>
       </c>
       <c r="H93" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="94" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B94" t="s">
-        <v>279</v>
+        <v>199</v>
       </c>
       <c r="C94" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D94" t="s">
         <v>23</v>
@@ -6072,15 +6133,15 @@
         <v>24</v>
       </c>
       <c r="H94" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="95" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B95" t="s">
-        <v>280</v>
+        <v>198</v>
       </c>
       <c r="C95" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="D95" t="s">
         <v>14</v>
@@ -6095,15 +6156,15 @@
         <v>24</v>
       </c>
       <c r="H95" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="96" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B96" t="s">
-        <v>281</v>
+        <v>197</v>
       </c>
       <c r="C96" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="D96" t="s">
         <v>14</v>
@@ -6118,15 +6179,15 @@
         <v>24</v>
       </c>
       <c r="H96" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="97" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B97" t="s">
-        <v>282</v>
+        <v>196</v>
       </c>
       <c r="C97" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D97" t="s">
         <v>14</v>
@@ -6141,15 +6202,15 @@
         <v>24</v>
       </c>
       <c r="H97" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="98" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B98" t="s">
-        <v>283</v>
+        <v>195</v>
       </c>
       <c r="C98" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D98" t="s">
         <v>14</v>
@@ -6169,10 +6230,10 @@
     </row>
     <row r="99" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B99" t="s">
-        <v>284</v>
+        <v>194</v>
       </c>
       <c r="C99" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="D99" t="s">
         <v>14</v>
@@ -6187,15 +6248,15 @@
         <v>24</v>
       </c>
       <c r="H99" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="100" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B100" t="s">
-        <v>285</v>
+        <v>193</v>
       </c>
       <c r="C100" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D100" t="s">
         <v>14</v>
@@ -6210,15 +6271,15 @@
         <v>24</v>
       </c>
       <c r="H100" t="s">
-        <v>204</v>
+        <v>187</v>
       </c>
     </row>
     <row r="101" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B101" t="s">
-        <v>286</v>
+        <v>192</v>
       </c>
       <c r="C101" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D101" t="s">
         <v>23</v>
@@ -6233,15 +6294,15 @@
         <v>24</v>
       </c>
       <c r="H101" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="102" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B102" t="s">
-        <v>287</v>
+        <v>191</v>
       </c>
       <c r="C102" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D102" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
0605 vue code arrangement and api
</commit_message>
<xml_diff>
--- a/backend/private/db/analysis/이미지_속성_최종.xlsx
+++ b/backend/private/db/analysis/이미지_속성_최종.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\study\Subject\Software Capstone\Project\문서\이미지 속성\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA72335-07F5-4BFE-92AE-A6620CB4AB0F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92F2EB41-5B56-4134-911F-7CFDF63375B8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4764" yWindow="2412" windowWidth="17280" windowHeight="8964" xr2:uid="{0D4B19A7-728F-4523-98BD-6CF286C421CB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{0D4B19A7-728F-4523-98BD-6CF286C421CB}"/>
   </bookViews>
   <sheets>
     <sheet name="setting" sheetId="3" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1425" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1425" uniqueCount="287">
   <si>
     <t>머리길이</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -747,18 +747,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">흰 피부 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">동양 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">귀여움 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>섹시</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -767,18 +755,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">장발 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">가르마 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">강아지 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>청순</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -907,10 +883,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>초이.jpg</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>채영.jpg</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -939,10 +911,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>전소민.jpg</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>이민정.jpg</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1200,6 +1168,18 @@
   </si>
   <si>
     <t>analysis_woman</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>귀여움</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>초아.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전소미.jpg</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1566,21 +1546,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBCEA11C-9251-44E7-AA41-F0DC5DACB4A0}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.3984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="B1" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
@@ -1588,7 +1569,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
@@ -1596,7 +1577,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
     </row>
   </sheetData>
@@ -1610,8 +1591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7DEA72E-EEE8-405E-88CB-70883EC1F59F}">
   <dimension ref="B1:H102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="F98" sqref="F98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -3939,7 +3920,7 @@
         <v>163</v>
       </c>
       <c r="F101" t="s">
-        <v>170</v>
+        <v>32</v>
       </c>
       <c r="G101" t="s">
         <v>164</v>
@@ -3982,8 +3963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F3E1D40-E48E-44C9-9049-1BB7413AF33F}">
   <dimension ref="B2:H102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -4022,7 +4003,7 @@
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B3" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="C3" t="s">
         <v>177</v>
@@ -4034,18 +4015,18 @@
         <v>31</v>
       </c>
       <c r="F3" t="s">
-        <v>178</v>
+        <v>32</v>
       </c>
       <c r="G3" t="s">
-        <v>179</v>
+        <v>16</v>
       </c>
       <c r="H3" t="s">
-        <v>180</v>
+        <v>284</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="C4" t="s">
         <v>177</v>
@@ -4063,12 +4044,12 @@
         <v>16</v>
       </c>
       <c r="H4" t="s">
-        <v>180</v>
+        <v>284</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="C5" t="s">
         <v>177</v>
@@ -4086,12 +4067,12 @@
         <v>16</v>
       </c>
       <c r="H5" t="s">
-        <v>180</v>
+        <v>284</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="C6" t="s">
         <v>177</v>
@@ -4109,12 +4090,12 @@
         <v>16</v>
       </c>
       <c r="H6" t="s">
-        <v>180</v>
+        <v>284</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B7" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="C7" t="s">
         <v>177</v>
@@ -4126,21 +4107,21 @@
         <v>27</v>
       </c>
       <c r="F7" t="s">
-        <v>178</v>
+        <v>32</v>
       </c>
       <c r="G7" t="s">
         <v>24</v>
       </c>
       <c r="H7" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="C8" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D8" t="s">
         <v>23</v>
@@ -4160,10 +4141,10 @@
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B9" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="C9" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D9" t="s">
         <v>14</v>
@@ -4178,12 +4159,12 @@
         <v>24</v>
       </c>
       <c r="H9" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B10" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="C10" t="s">
         <v>177</v>
@@ -4201,12 +4182,12 @@
         <v>24</v>
       </c>
       <c r="H10" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B11" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="C11" t="s">
         <v>177</v>
@@ -4224,15 +4205,15 @@
         <v>24</v>
       </c>
       <c r="H11" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B12" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="C12" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D12" t="s">
         <v>23</v>
@@ -4247,21 +4228,21 @@
         <v>24</v>
       </c>
       <c r="H12" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B13" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="C13" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="D13" t="s">
-        <v>184</v>
+        <v>14</v>
       </c>
       <c r="E13" t="s">
-        <v>185</v>
+        <v>31</v>
       </c>
       <c r="F13" t="s">
         <v>28</v>
@@ -4270,12 +4251,12 @@
         <v>24</v>
       </c>
       <c r="H13" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B14" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="C14" t="s">
         <v>177</v>
@@ -4293,12 +4274,12 @@
         <v>24</v>
       </c>
       <c r="H14" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B15" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="C15" t="s">
         <v>177</v>
@@ -4321,7 +4302,7 @@
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B16" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="C16" t="s">
         <v>177</v>
@@ -4339,12 +4320,12 @@
         <v>24</v>
       </c>
       <c r="H16" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B17" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="C17" t="s">
         <v>177</v>
@@ -4362,12 +4343,12 @@
         <v>16</v>
       </c>
       <c r="H17" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B18" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="C18" t="s">
         <v>177</v>
@@ -4385,12 +4366,12 @@
         <v>16</v>
       </c>
       <c r="H18" t="s">
-        <v>180</v>
+        <v>284</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B19" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="C19" t="s">
         <v>177</v>
@@ -4408,12 +4389,12 @@
         <v>16</v>
       </c>
       <c r="H19" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B20" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="C20" t="s">
         <v>177</v>
@@ -4431,12 +4412,12 @@
         <v>16</v>
       </c>
       <c r="H20" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B21" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="C21" t="s">
         <v>177</v>
@@ -4454,12 +4435,12 @@
         <v>16</v>
       </c>
       <c r="H21" t="s">
-        <v>180</v>
+        <v>284</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B22" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="C22" t="s">
         <v>177</v>
@@ -4477,12 +4458,12 @@
         <v>16</v>
       </c>
       <c r="H22" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B23" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="C23" t="s">
         <v>177</v>
@@ -4500,12 +4481,12 @@
         <v>16</v>
       </c>
       <c r="H23" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B24" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="C24" t="s">
         <v>177</v>
@@ -4523,12 +4504,12 @@
         <v>16</v>
       </c>
       <c r="H24" t="s">
-        <v>180</v>
+        <v>284</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B25" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="C25" t="s">
         <v>177</v>
@@ -4546,12 +4527,12 @@
         <v>16</v>
       </c>
       <c r="H25" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B26" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="C26" t="s">
         <v>177</v>
@@ -4569,12 +4550,12 @@
         <v>16</v>
       </c>
       <c r="H26" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B27" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="C27" t="s">
         <v>177</v>
@@ -4592,12 +4573,12 @@
         <v>16</v>
       </c>
       <c r="H27" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B28" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="C28" t="s">
         <v>177</v>
@@ -4615,12 +4596,12 @@
         <v>16</v>
       </c>
       <c r="H28" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B29" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="C29" t="s">
         <v>177</v>
@@ -4638,12 +4619,12 @@
         <v>16</v>
       </c>
       <c r="H29" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B30" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="C30" t="s">
         <v>177</v>
@@ -4661,12 +4642,12 @@
         <v>16</v>
       </c>
       <c r="H30" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B31" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="C31" t="s">
         <v>177</v>
@@ -4684,12 +4665,12 @@
         <v>16</v>
       </c>
       <c r="H31" t="s">
-        <v>180</v>
+        <v>284</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B32" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="C32" t="s">
         <v>177</v>
@@ -4707,12 +4688,12 @@
         <v>16</v>
       </c>
       <c r="H32" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B33" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="C33" t="s">
         <v>177</v>
@@ -4730,12 +4711,12 @@
         <v>16</v>
       </c>
       <c r="H33" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B34" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="C34" t="s">
         <v>15</v>
@@ -4753,12 +4734,12 @@
         <v>16</v>
       </c>
       <c r="H34" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B35" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="C35" t="s">
         <v>177</v>
@@ -4776,12 +4757,12 @@
         <v>16</v>
       </c>
       <c r="H35" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B36" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="C36" t="s">
         <v>177</v>
@@ -4804,10 +4785,10 @@
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B37" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="C37" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D37" t="s">
         <v>23</v>
@@ -4822,15 +4803,15 @@
         <v>24</v>
       </c>
       <c r="H37" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B38" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="C38" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D38" t="s">
         <v>23</v>
@@ -4845,12 +4826,12 @@
         <v>24</v>
       </c>
       <c r="H38" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B39" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="C39" t="s">
         <v>177</v>
@@ -4868,15 +4849,15 @@
         <v>24</v>
       </c>
       <c r="H39" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B40" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="C40" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D40" t="s">
         <v>21</v>
@@ -4896,7 +4877,7 @@
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B41" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="C41" t="s">
         <v>177</v>
@@ -4914,12 +4895,12 @@
         <v>24</v>
       </c>
       <c r="H41" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B42" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="C42" t="s">
         <v>177</v>
@@ -4942,7 +4923,7 @@
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B43" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="C43" t="s">
         <v>177</v>
@@ -4960,12 +4941,12 @@
         <v>24</v>
       </c>
       <c r="H43" t="s">
-        <v>180</v>
+        <v>284</v>
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B44" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="C44" t="s">
         <v>177</v>
@@ -4983,15 +4964,15 @@
         <v>24</v>
       </c>
       <c r="H44" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B45" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="C45" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D45" t="s">
         <v>23</v>
@@ -5006,12 +4987,12 @@
         <v>24</v>
       </c>
       <c r="H45" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B46" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="C46" t="s">
         <v>177</v>
@@ -5029,15 +5010,15 @@
         <v>24</v>
       </c>
       <c r="H46" t="s">
-        <v>180</v>
+        <v>284</v>
       </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B47" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="C47" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="D47" t="s">
         <v>14</v>
@@ -5052,15 +5033,15 @@
         <v>24</v>
       </c>
       <c r="H47" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B48" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="C48" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D48" t="s">
         <v>21</v>
@@ -5075,15 +5056,15 @@
         <v>24</v>
       </c>
       <c r="H48" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B49" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="C49" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="D49" t="s">
         <v>23</v>
@@ -5098,12 +5079,12 @@
         <v>24</v>
       </c>
       <c r="H49" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B50" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="C50" t="s">
         <v>177</v>
@@ -5121,12 +5102,12 @@
         <v>24</v>
       </c>
       <c r="H50" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B51" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="C51" t="s">
         <v>177</v>
@@ -5144,12 +5125,12 @@
         <v>24</v>
       </c>
       <c r="H51" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B52" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="C52" t="s">
         <v>177</v>
@@ -5167,12 +5148,12 @@
         <v>24</v>
       </c>
       <c r="H52" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B53" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="C53" t="s">
         <v>177</v>
@@ -5190,12 +5171,12 @@
         <v>24</v>
       </c>
       <c r="H53" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B54" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="C54" t="s">
         <v>177</v>
@@ -5213,12 +5194,12 @@
         <v>16</v>
       </c>
       <c r="H54" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B55" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="C55" t="s">
         <v>177</v>
@@ -5236,12 +5217,12 @@
         <v>16</v>
       </c>
       <c r="H55" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B56" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="C56" t="s">
         <v>177</v>
@@ -5259,12 +5240,12 @@
         <v>16</v>
       </c>
       <c r="H56" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="57" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B57" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="C57" t="s">
         <v>177</v>
@@ -5282,12 +5263,12 @@
         <v>16</v>
       </c>
       <c r="H57" t="s">
-        <v>180</v>
+        <v>284</v>
       </c>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B58" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="C58" t="s">
         <v>177</v>
@@ -5305,12 +5286,12 @@
         <v>16</v>
       </c>
       <c r="H58" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B59" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="C59" t="s">
         <v>177</v>
@@ -5328,12 +5309,12 @@
         <v>16</v>
       </c>
       <c r="H59" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B60" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="C60" t="s">
         <v>177</v>
@@ -5351,15 +5332,15 @@
         <v>16</v>
       </c>
       <c r="H60" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B61" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="C61" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D61" t="s">
         <v>14</v>
@@ -5374,12 +5355,12 @@
         <v>16</v>
       </c>
       <c r="H61" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B62" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="C62" t="s">
         <v>177</v>
@@ -5397,15 +5378,15 @@
         <v>16</v>
       </c>
       <c r="H62" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B63" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="C63" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="D63" t="s">
         <v>14</v>
@@ -5420,12 +5401,12 @@
         <v>16</v>
       </c>
       <c r="H63" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="64" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B64" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="C64" t="s">
         <v>177</v>
@@ -5443,12 +5424,12 @@
         <v>16</v>
       </c>
       <c r="H64" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="65" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B65" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="C65" t="s">
         <v>177</v>
@@ -5466,12 +5447,12 @@
         <v>16</v>
       </c>
       <c r="H65" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="66" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B66" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="C66" t="s">
         <v>177</v>
@@ -5489,15 +5470,15 @@
         <v>16</v>
       </c>
       <c r="H66" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="67" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B67" t="s">
-        <v>226</v>
+        <v>286</v>
       </c>
       <c r="C67" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D67" t="s">
         <v>14</v>
@@ -5512,12 +5493,12 @@
         <v>16</v>
       </c>
       <c r="H67" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="68" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B68" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="C68" t="s">
         <v>177</v>
@@ -5535,15 +5516,15 @@
         <v>16</v>
       </c>
       <c r="H68" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="69" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B69" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="C69" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D69" t="s">
         <v>21</v>
@@ -5558,12 +5539,12 @@
         <v>16</v>
       </c>
       <c r="H69" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="70" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B70" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="C70" t="s">
         <v>177</v>
@@ -5581,12 +5562,12 @@
         <v>16</v>
       </c>
       <c r="H70" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="71" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B71" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="C71" t="s">
         <v>177</v>
@@ -5604,12 +5585,12 @@
         <v>16</v>
       </c>
       <c r="H71" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="72" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B72" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="C72" t="s">
         <v>177</v>
@@ -5627,12 +5608,12 @@
         <v>16</v>
       </c>
       <c r="H72" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="73" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B73" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="C73" t="s">
         <v>177</v>
@@ -5650,12 +5631,12 @@
         <v>16</v>
       </c>
       <c r="H73" t="s">
-        <v>180</v>
+        <v>284</v>
       </c>
     </row>
     <row r="74" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B74" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="C74" t="s">
         <v>177</v>
@@ -5673,15 +5654,15 @@
         <v>16</v>
       </c>
       <c r="H74" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="75" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B75" t="s">
-        <v>218</v>
+        <v>285</v>
       </c>
       <c r="C75" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D75" t="s">
         <v>14</v>
@@ -5696,12 +5677,12 @@
         <v>16</v>
       </c>
       <c r="H75" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="76" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B76" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="C76" t="s">
         <v>177</v>
@@ -5719,12 +5700,12 @@
         <v>16</v>
       </c>
       <c r="H76" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="77" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B77" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="C77" t="s">
         <v>177</v>
@@ -5742,12 +5723,12 @@
         <v>16</v>
       </c>
       <c r="H77" t="s">
-        <v>180</v>
+        <v>284</v>
       </c>
     </row>
     <row r="78" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B78" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="C78" t="s">
         <v>177</v>
@@ -5765,12 +5746,12 @@
         <v>16</v>
       </c>
       <c r="H78" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="79" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B79" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="C79" t="s">
         <v>177</v>
@@ -5788,12 +5769,12 @@
         <v>16</v>
       </c>
       <c r="H79" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="80" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B80" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="C80" t="s">
         <v>177</v>
@@ -5811,12 +5792,12 @@
         <v>24</v>
       </c>
       <c r="H80" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="81" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B81" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="C81" t="s">
         <v>177</v>
@@ -5834,12 +5815,12 @@
         <v>24</v>
       </c>
       <c r="H81" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="82" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B82" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="C82" t="s">
         <v>177</v>
@@ -5857,12 +5838,12 @@
         <v>24</v>
       </c>
       <c r="H82" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="83" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B83" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="C83" t="s">
         <v>177</v>
@@ -5880,12 +5861,12 @@
         <v>24</v>
       </c>
       <c r="H83" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="84" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B84" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="C84" t="s">
         <v>177</v>
@@ -5903,15 +5884,15 @@
         <v>24</v>
       </c>
       <c r="H84" t="s">
-        <v>180</v>
+        <v>284</v>
       </c>
     </row>
     <row r="85" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B85" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="C85" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D85" t="s">
         <v>14</v>
@@ -5926,12 +5907,12 @@
         <v>24</v>
       </c>
       <c r="H85" t="s">
-        <v>180</v>
+        <v>284</v>
       </c>
     </row>
     <row r="86" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B86" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="C86" t="s">
         <v>177</v>
@@ -5949,12 +5930,12 @@
         <v>24</v>
       </c>
       <c r="H86" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="87" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B87" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="C87" t="s">
         <v>177</v>
@@ -5972,12 +5953,12 @@
         <v>24</v>
       </c>
       <c r="H87" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="88" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B88" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="C88" t="s">
         <v>177</v>
@@ -5995,12 +5976,12 @@
         <v>24</v>
       </c>
       <c r="H88" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="89" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B89" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="C89" t="s">
         <v>177</v>
@@ -6018,12 +5999,12 @@
         <v>24</v>
       </c>
       <c r="H89" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="90" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B90" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="C90" t="s">
         <v>177</v>
@@ -6041,12 +6022,12 @@
         <v>24</v>
       </c>
       <c r="H90" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="91" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B91" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="C91" t="s">
         <v>177</v>
@@ -6064,12 +6045,12 @@
         <v>24</v>
       </c>
       <c r="H91" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="92" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B92" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="C92" t="s">
         <v>177</v>
@@ -6087,12 +6068,12 @@
         <v>24</v>
       </c>
       <c r="H92" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="93" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B93" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="C93" t="s">
         <v>177</v>
@@ -6110,12 +6091,12 @@
         <v>24</v>
       </c>
       <c r="H93" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="94" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B94" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C94" t="s">
         <v>177</v>
@@ -6133,15 +6114,15 @@
         <v>24</v>
       </c>
       <c r="H94" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="95" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B95" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="C95" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D95" t="s">
         <v>14</v>
@@ -6156,15 +6137,15 @@
         <v>24</v>
       </c>
       <c r="H95" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="96" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B96" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="C96" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D96" t="s">
         <v>14</v>
@@ -6179,12 +6160,12 @@
         <v>24</v>
       </c>
       <c r="H96" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="97" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B97" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="C97" t="s">
         <v>177</v>
@@ -6202,12 +6183,12 @@
         <v>24</v>
       </c>
       <c r="H97" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="98" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B98" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="C98" t="s">
         <v>177</v>
@@ -6230,10 +6211,10 @@
     </row>
     <row r="99" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B99" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="C99" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D99" t="s">
         <v>14</v>
@@ -6248,12 +6229,12 @@
         <v>24</v>
       </c>
       <c r="H99" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="100" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B100" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="C100" t="s">
         <v>177</v>
@@ -6271,12 +6252,12 @@
         <v>24</v>
       </c>
       <c r="H100" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="101" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B101" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="C101" t="s">
         <v>177</v>
@@ -6294,12 +6275,12 @@
         <v>24</v>
       </c>
       <c r="H101" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="102" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B102" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="C102" t="s">
         <v>177</v>

</xml_diff>

<commit_message>
0607 result, modify api, menu reload
</commit_message>
<xml_diff>
--- a/backend/private/db/analysis/이미지_속성_최종.xlsx
+++ b/backend/private/db/analysis/이미지_속성_최종.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\study\Subject\Software Capstone\Project\문서\이미지 속성\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92F2EB41-5B56-4134-911F-7CFDF63375B8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B31D90B5-F35F-4EC4-8E99-E3E76C470F39}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{0D4B19A7-728F-4523-98BD-6CF286C421CB}"/>
+    <workbookView xWindow="5760" yWindow="120" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{0D4B19A7-728F-4523-98BD-6CF286C421CB}"/>
   </bookViews>
   <sheets>
     <sheet name="setting" sheetId="3" r:id="rId1"/>
@@ -1023,10 +1023,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>안렉산드라다드다리오.jpg</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>안젤리나졸리.jpg</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1180,6 +1176,10 @@
   </si>
   <si>
     <t>전소미.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>알렉산드라다드다리오.jpg</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1558,10 +1558,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
@@ -1569,7 +1569,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
@@ -1577,7 +1577,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -3963,8 +3963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F3E1D40-E48E-44C9-9049-1BB7413AF33F}">
   <dimension ref="B2:H102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="E59" sqref="E59"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -4021,7 +4021,7 @@
         <v>16</v>
       </c>
       <c r="H3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.4">
@@ -4044,7 +4044,7 @@
         <v>16</v>
       </c>
       <c r="H4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.4">
@@ -4067,7 +4067,7 @@
         <v>16</v>
       </c>
       <c r="H5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.4">
@@ -4090,7 +4090,7 @@
         <v>16</v>
       </c>
       <c r="H6" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.4">
@@ -4187,7 +4187,7 @@
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C11" t="s">
         <v>177</v>
@@ -4210,7 +4210,7 @@
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B12" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C12" t="s">
         <v>179</v>
@@ -4233,7 +4233,7 @@
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C13" t="s">
         <v>177</v>
@@ -4256,7 +4256,7 @@
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B14" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C14" t="s">
         <v>177</v>
@@ -4279,7 +4279,7 @@
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B15" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C15" t="s">
         <v>177</v>
@@ -4302,7 +4302,7 @@
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B16" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C16" t="s">
         <v>177</v>
@@ -4325,7 +4325,7 @@
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B17" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C17" t="s">
         <v>177</v>
@@ -4348,7 +4348,7 @@
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B18" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C18" t="s">
         <v>177</v>
@@ -4366,12 +4366,12 @@
         <v>16</v>
       </c>
       <c r="H18" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B19" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C19" t="s">
         <v>177</v>
@@ -4394,7 +4394,7 @@
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B20" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C20" t="s">
         <v>177</v>
@@ -4417,7 +4417,7 @@
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B21" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C21" t="s">
         <v>177</v>
@@ -4435,12 +4435,12 @@
         <v>16</v>
       </c>
       <c r="H21" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B22" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C22" t="s">
         <v>177</v>
@@ -4463,7 +4463,7 @@
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B23" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C23" t="s">
         <v>177</v>
@@ -4486,7 +4486,7 @@
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B24" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C24" t="s">
         <v>177</v>
@@ -4504,12 +4504,12 @@
         <v>16</v>
       </c>
       <c r="H24" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B25" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C25" t="s">
         <v>177</v>
@@ -4532,7 +4532,7 @@
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B26" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C26" t="s">
         <v>177</v>
@@ -4555,7 +4555,7 @@
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B27" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C27" t="s">
         <v>177</v>
@@ -4578,7 +4578,7 @@
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B28" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C28" t="s">
         <v>177</v>
@@ -4601,7 +4601,7 @@
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B29" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C29" t="s">
         <v>177</v>
@@ -4624,7 +4624,7 @@
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B30" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C30" t="s">
         <v>177</v>
@@ -4647,7 +4647,7 @@
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B31" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C31" t="s">
         <v>177</v>
@@ -4665,12 +4665,12 @@
         <v>16</v>
       </c>
       <c r="H31" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B32" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C32" t="s">
         <v>177</v>
@@ -4693,7 +4693,7 @@
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B33" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C33" t="s">
         <v>177</v>
@@ -4716,7 +4716,7 @@
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B34" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C34" t="s">
         <v>15</v>
@@ -4739,7 +4739,7 @@
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B35" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C35" t="s">
         <v>177</v>
@@ -4762,7 +4762,7 @@
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B36" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C36" t="s">
         <v>177</v>
@@ -4785,7 +4785,7 @@
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B37" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C37" t="s">
         <v>179</v>
@@ -4808,7 +4808,7 @@
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B38" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C38" t="s">
         <v>179</v>
@@ -4831,7 +4831,7 @@
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B39" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C39" t="s">
         <v>177</v>
@@ -4854,7 +4854,7 @@
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B40" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C40" t="s">
         <v>179</v>
@@ -4877,7 +4877,7 @@
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B41" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C41" t="s">
         <v>177</v>
@@ -4900,7 +4900,7 @@
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B42" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C42" t="s">
         <v>177</v>
@@ -4923,7 +4923,7 @@
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B43" t="s">
-        <v>247</v>
+        <v>286</v>
       </c>
       <c r="C43" t="s">
         <v>177</v>
@@ -4941,7 +4941,7 @@
         <v>24</v>
       </c>
       <c r="H43" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.4">
@@ -5010,7 +5010,7 @@
         <v>24</v>
       </c>
       <c r="H46" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.4">
@@ -5263,7 +5263,7 @@
         <v>16</v>
       </c>
       <c r="H57" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.4">
@@ -5475,7 +5475,7 @@
     </row>
     <row r="67" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B67" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C67" t="s">
         <v>179</v>
@@ -5631,7 +5631,7 @@
         <v>16</v>
       </c>
       <c r="H73" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="74" spans="2:8" x14ac:dyDescent="0.4">
@@ -5659,7 +5659,7 @@
     </row>
     <row r="75" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B75" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C75" t="s">
         <v>179</v>
@@ -5723,7 +5723,7 @@
         <v>16</v>
       </c>
       <c r="H77" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="78" spans="2:8" x14ac:dyDescent="0.4">
@@ -5884,7 +5884,7 @@
         <v>24</v>
       </c>
       <c r="H84" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="85" spans="2:8" x14ac:dyDescent="0.4">
@@ -5907,7 +5907,7 @@
         <v>24</v>
       </c>
       <c r="H85" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="86" spans="2:8" x14ac:dyDescent="0.4">

</xml_diff>